<commit_message>
notebook : tableau des infos de chaque base
</commit_message>
<xml_diff>
--- a/DescData1.1.xlsx
+++ b/DescData1.1.xlsx
@@ -219,9 +219,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Country Code [PK]</t>
   </si>
   <si>
@@ -244,13 +241,16 @@
   </si>
   <si>
     <t>SeriesCode [PFK]</t>
+  </si>
+  <si>
+    <t>Year [PK]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +273,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -533,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,12 +548,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -568,29 +568,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -604,12 +583,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,20 +647,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>816428</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>775607</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>617764</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>232682</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>115661</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="4" name="Image 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -670,8 +680,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="15825107" y="2190750"/>
-          <a:ext cx="6781800" cy="3541939"/>
+          <a:off x="10327821" y="2735036"/>
+          <a:ext cx="6560004" cy="3218089"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -980,19 +990,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N36"/>
+  <dimension ref="A2:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
     <col min="6" max="6" width="42.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" customWidth="1"/>
@@ -1007,52 +1017,52 @@
   <sheetData>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="25" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="47"/>
+      <c r="H3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="31" t="s">
+      <c r="I3" s="47"/>
+      <c r="J3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="27"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="37">
         <v>886930</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="24">
+      <c r="C4" s="39"/>
+      <c r="D4" s="37">
         <v>241</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="24">
+      <c r="E4" s="38"/>
+      <c r="F4" s="37">
         <v>3665</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="24">
+      <c r="G4" s="38"/>
+      <c r="H4" s="37">
         <v>613</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="32">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39">
         <v>643638</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="38"/>
       <c r="L4" t="s">
         <v>10</v>
       </c>
@@ -1061,55 +1071,65 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="40">
         <v>69</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="46">
+      <c r="C5" s="41"/>
+      <c r="D5" s="40">
         <v>31</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="46">
+      <c r="E5" s="41"/>
+      <c r="F5" s="40">
         <v>20</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="46">
+      <c r="G5" s="41"/>
+      <c r="H5" s="40">
         <v>3</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="46">
+      <c r="I5" s="41"/>
+      <c r="J5" s="40">
         <v>4</v>
       </c>
-      <c r="K5" s="47"/>
+      <c r="K5" s="41"/>
       <c r="M5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="43"/>
+      <c r="B6" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="24">
+        <v>242</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="3">
+        <v>241</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3665</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" s="3"/>
+      <c r="I6" s="3">
+        <v>211</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="3">
+        <v>239</v>
+      </c>
       <c r="L6" t="s">
         <v>13</v>
       </c>
@@ -1118,53 +1138,73 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="9" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="25">
+        <v>242</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="22">
+        <v>241</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="29"/>
+      <c r="G7" s="35">
+        <v>37</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="4">
+        <v>21</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="23">
+        <v>1558</v>
+      </c>
       <c r="M7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="9" t="s">
+      <c r="A8" s="43"/>
+      <c r="B8" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="26">
+        <v>3665</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="22">
+        <v>241</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="36">
+        <v>3665</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K8" s="15"/>
+      <c r="I8" s="13">
+        <v>97</v>
+      </c>
+      <c r="J8" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="13">
+        <v>56</v>
+      </c>
       <c r="L8" t="s">
         <v>14</v>
       </c>
@@ -1176,25 +1216,33 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="9" t="s">
+      <c r="A9" s="43"/>
+      <c r="B9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="27">
+        <v>3665</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="22">
+        <v>241</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="35">
+        <v>1170</v>
+      </c>
+      <c r="H9" s="6"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="13">
+        <v>9102</v>
+      </c>
       <c r="M9" t="s">
         <v>16</v>
       </c>
@@ -1203,22 +1251,26 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="11" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="22">
+        <v>239</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="35">
+        <v>2060</v>
+      </c>
+      <c r="H10" s="6"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="22"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="2"/>
       <c r="M10" t="s">
         <v>17</v>
@@ -1228,436 +1280,573 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="43"/>
+      <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="13">
+        <v>153</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="13">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="22"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="40" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="32">
+        <v>132</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="13">
+        <v>2</v>
+      </c>
+      <c r="H12" s="6"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="20"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="9" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="22">
+        <v>8</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="13">
+        <v>5</v>
+      </c>
+      <c r="H13" s="6"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="22"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="11" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="40" t="s">
+      <c r="E14" s="13">
+        <v>6</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="32">
+        <v>15</v>
+      </c>
+      <c r="H14" s="6"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="22"/>
+      <c r="J14" s="20"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="11" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="11" t="s">
+      <c r="E15" s="13">
+        <v>241</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="13">
+        <v>4</v>
+      </c>
+      <c r="H15" s="6"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="22"/>
+      <c r="J15" s="20"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="11" t="s">
+      <c r="A16" s="43"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="40" t="s">
+      <c r="E16" s="13">
+        <v>44</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="32">
+        <v>10</v>
+      </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="22"/>
+      <c r="J16" s="20"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="11" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="40" t="s">
+      <c r="E17" s="13">
+        <v>12</v>
+      </c>
+      <c r="F17" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="32">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="22"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="11" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="40" t="s">
+      <c r="E18" s="13">
+        <v>3</v>
+      </c>
+      <c r="F18" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="41"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="32">
+        <v>9</v>
+      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="22"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="11" t="s">
+      <c r="A19" s="43"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="40" t="s">
+      <c r="E19" s="13">
+        <v>4</v>
+      </c>
+      <c r="F19" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="41"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="32">
+        <v>31</v>
+      </c>
+      <c r="H19" s="6"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="22"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="11" t="s">
+      <c r="A20" s="43"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="40" t="s">
+      <c r="E20" s="13">
+        <v>3</v>
+      </c>
+      <c r="F20" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="32">
+        <v>3</v>
+      </c>
+      <c r="H20" s="6"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="22"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="11" t="s">
+      <c r="A21" s="43"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="40" t="s">
+      <c r="E21" s="13">
+        <v>4</v>
+      </c>
+      <c r="F21" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="41"/>
-      <c r="H21" s="8"/>
+      <c r="G21" s="32">
+        <v>2</v>
+      </c>
+      <c r="H21" s="6"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="22"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="11" t="s">
+      <c r="A22" s="43"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="40" t="s">
+      <c r="E22" s="13">
+        <v>33</v>
+      </c>
+      <c r="F22" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="8"/>
+      <c r="G22" s="32">
+        <v>2</v>
+      </c>
+      <c r="H22" s="6"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="22"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="11" t="s">
+      <c r="A23" s="43"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="40" t="s">
+      <c r="E23" s="13">
+        <v>4</v>
+      </c>
+      <c r="F23" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="32">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="22"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="11" t="s">
+      <c r="A24" s="43"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="40" t="s">
+      <c r="E24" s="13">
+        <v>2</v>
+      </c>
+      <c r="F24" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="41"/>
-      <c r="H24" s="8"/>
+      <c r="G24" s="32">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="22"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="11" t="s">
+      <c r="A25" s="43"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="40" t="s">
+      <c r="E25" s="13">
+        <v>4</v>
+      </c>
+      <c r="F25" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="8"/>
+      <c r="G25" s="32">
+        <v>1</v>
+      </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="22"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="11" t="s">
+      <c r="A26" s="43"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="8"/>
+      <c r="E26" s="13">
+        <v>3</v>
+      </c>
+      <c r="F26" s="6"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="8"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="22"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="11" t="s">
+      <c r="A27" s="43"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="8"/>
+      <c r="E27" s="13">
+        <v>3</v>
+      </c>
+      <c r="F27" s="6"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="8"/>
+      <c r="H27" s="6"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="22"/>
+      <c r="J27" s="20"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="11" t="s">
+      <c r="A28" s="43"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="8"/>
+      <c r="E28" s="13">
+        <v>3</v>
+      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="8"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="22"/>
+      <c r="J28" s="20"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="11" t="s">
+      <c r="A29" s="43"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="8"/>
+      <c r="E29" s="13">
+        <v>28</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="8"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="22"/>
+      <c r="J29" s="20"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="11" t="s">
+      <c r="A30" s="43"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="8"/>
+      <c r="E30" s="13">
+        <v>61</v>
+      </c>
+      <c r="F30" s="6"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="8"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="22"/>
+      <c r="J30" s="20"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="11" t="s">
+      <c r="A31" s="43"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="8"/>
+      <c r="E31" s="13">
+        <v>76</v>
+      </c>
+      <c r="F31" s="6"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="8"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="22"/>
+      <c r="J31" s="20"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="11" t="s">
+      <c r="A32" s="43"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="8"/>
+      <c r="E32" s="13">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="6"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="22"/>
+      <c r="J32" s="20"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="11" t="s">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="43"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="8"/>
+      <c r="E33" s="13">
+        <v>36</v>
+      </c>
+      <c r="F33" s="6"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="8"/>
+      <c r="H33" s="6"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="22"/>
+      <c r="J33" s="20"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="11" t="s">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="8"/>
+      <c r="E34" s="13">
+        <v>12</v>
+      </c>
+      <c r="F34" s="6"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="8"/>
+      <c r="H34" s="6"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="22"/>
+      <c r="J34" s="20"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="11" t="s">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="8"/>
+      <c r="E35" s="13">
+        <v>14</v>
+      </c>
+      <c r="F35" s="6"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="8"/>
+      <c r="H35" s="6"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="22"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="42" t="s">
+    <row r="36" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="44"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="43"/>
-      <c r="F36" s="12"/>
+      <c r="E36" s="34">
+        <v>21</v>
+      </c>
+      <c r="F36" s="10"/>
       <c r="G36" s="5"/>
-      <c r="H36" s="12"/>
+      <c r="H36" s="10"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="23"/>
+      <c r="J36" s="21"/>
       <c r="K36" s="5"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D40" s="48">
+        <v>3665</v>
+      </c>
+      <c r="E40">
+        <v>37</v>
+      </c>
+      <c r="F40">
+        <v>3665</v>
+      </c>
+      <c r="G40">
+        <v>1170</v>
+      </c>
+      <c r="H40">
+        <v>2060</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>5</v>
+      </c>
+      <c r="L40">
+        <v>15</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>10</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>9</v>
+      </c>
+      <c r="Q40">
+        <v>31</v>
+      </c>
+      <c r="R40">
+        <v>3</v>
+      </c>
+      <c r="S40">
+        <v>2</v>
+      </c>
+      <c r="T40">
+        <v>2</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="A5:A36"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
@@ -1667,6 +1856,13 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1676,13 +1872,267 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B7:AF39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9:AA39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B7" s="48">
+        <v>241</v>
+      </c>
+      <c r="C7">
+        <v>241</v>
+      </c>
+      <c r="D7">
+        <v>241</v>
+      </c>
+      <c r="E7">
+        <v>241</v>
+      </c>
+      <c r="F7">
+        <v>239</v>
+      </c>
+      <c r="G7">
+        <v>153</v>
+      </c>
+      <c r="H7">
+        <v>132</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>241</v>
+      </c>
+      <c r="L7">
+        <v>44</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>33</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>3</v>
+      </c>
+      <c r="Y7">
+        <v>28</v>
+      </c>
+      <c r="Z7">
+        <v>61</v>
+      </c>
+      <c r="AA7">
+        <v>76</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>36</v>
+      </c>
+      <c r="AD7">
+        <v>12</v>
+      </c>
+      <c r="AE7">
+        <v>14</v>
+      </c>
+      <c r="AF7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA9" s="48">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA10">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA11">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA12">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA13">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA14">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="AA16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA18">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA19">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA34">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA39">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
mise en page du notebook + rédaction
</commit_message>
<xml_diff>
--- a/DescData1.1.xlsx
+++ b/DescData1.1.xlsx
@@ -583,21 +583,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -606,6 +595,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,10 +611,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,7 +993,7 @@
   <dimension ref="A2:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,51 +1018,51 @@
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="45" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="46" t="s">
+      <c r="I3" s="46"/>
+      <c r="J3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="47"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="42">
         <v>886930</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="37">
+      <c r="C4" s="43"/>
+      <c r="D4" s="42">
         <v>241</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="37">
+      <c r="E4" s="47"/>
+      <c r="F4" s="42">
         <v>3665</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="37">
+      <c r="G4" s="47"/>
+      <c r="H4" s="42">
         <v>613</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39">
+      <c r="I4" s="47"/>
+      <c r="J4" s="43">
         <v>643638</v>
       </c>
-      <c r="K4" s="38"/>
+      <c r="K4" s="47"/>
       <c r="L4" t="s">
         <v>10</v>
       </c>
@@ -1071,35 +1071,35 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="48">
         <v>69</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="40">
+      <c r="C5" s="49"/>
+      <c r="D5" s="48">
         <v>31</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="40">
+      <c r="E5" s="49"/>
+      <c r="F5" s="48">
         <v>20</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="40">
+      <c r="G5" s="49"/>
+      <c r="H5" s="48">
         <v>3</v>
       </c>
-      <c r="I5" s="41"/>
-      <c r="J5" s="40">
+      <c r="I5" s="49"/>
+      <c r="J5" s="48">
         <v>4</v>
       </c>
-      <c r="K5" s="41"/>
+      <c r="K5" s="49"/>
       <c r="M5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="7" t="s">
         <v>72</v>
       </c>
@@ -1138,7 +1138,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="8" t="s">
         <v>68</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="16" t="s">
         <v>71</v>
       </c>
@@ -1199,7 +1199,7 @@
       <c r="I8" s="13">
         <v>97</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="38" t="s">
         <v>75</v>
       </c>
       <c r="K8" s="13">
@@ -1216,7 +1216,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="14" t="s">
         <v>69</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="6"/>
       <c r="C12" s="29"/>
       <c r="D12" s="31" t="s">
@@ -1324,7 +1324,7 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="6"/>
       <c r="C13" s="29"/>
       <c r="D13" s="7" t="s">
@@ -1345,7 +1345,7 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="6"/>
       <c r="C14" s="29"/>
       <c r="D14" s="9" t="s">
@@ -1366,7 +1366,7 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="6"/>
       <c r="C15" s="29"/>
       <c r="D15" s="9" t="s">
@@ -1387,7 +1387,7 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="6"/>
       <c r="C16" s="29"/>
       <c r="D16" s="9" t="s">
@@ -1408,7 +1408,7 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="6"/>
       <c r="C17" s="29"/>
       <c r="D17" s="9" t="s">
@@ -1429,7 +1429,7 @@
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="6"/>
       <c r="C18" s="29"/>
       <c r="D18" s="9" t="s">
@@ -1450,7 +1450,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="6"/>
       <c r="C19" s="29"/>
       <c r="D19" s="9" t="s">
@@ -1471,7 +1471,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="6"/>
       <c r="C20" s="29"/>
       <c r="D20" s="9" t="s">
@@ -1492,7 +1492,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="6"/>
       <c r="C21" s="29"/>
       <c r="D21" s="9" t="s">
@@ -1513,7 +1513,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="6"/>
       <c r="C22" s="29"/>
       <c r="D22" s="9" t="s">
@@ -1534,7 +1534,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="6"/>
       <c r="C23" s="29"/>
       <c r="D23" s="9" t="s">
@@ -1555,7 +1555,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="6"/>
       <c r="C24" s="29"/>
       <c r="D24" s="9" t="s">
@@ -1576,7 +1576,7 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="6"/>
       <c r="C25" s="29"/>
       <c r="D25" s="9" t="s">
@@ -1597,7 +1597,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="6"/>
       <c r="C26" s="29"/>
       <c r="D26" s="9" t="s">
@@ -1614,7 +1614,7 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="6"/>
       <c r="C27" s="29"/>
       <c r="D27" s="9" t="s">
@@ -1631,7 +1631,7 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="6"/>
       <c r="C28" s="29"/>
       <c r="D28" s="9" t="s">
@@ -1648,7 +1648,7 @@
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="6"/>
       <c r="C29" s="29"/>
       <c r="D29" s="9" t="s">
@@ -1665,7 +1665,7 @@
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="6"/>
       <c r="C30" s="29"/>
       <c r="D30" s="9" t="s">
@@ -1682,7 +1682,7 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="6"/>
       <c r="C31" s="29"/>
       <c r="D31" s="9" t="s">
@@ -1699,7 +1699,7 @@
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="6"/>
       <c r="C32" s="29"/>
       <c r="D32" s="9" t="s">
@@ -1716,7 +1716,7 @@
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="6"/>
       <c r="C33" s="29"/>
       <c r="D33" s="9" t="s">
@@ -1733,7 +1733,7 @@
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="6"/>
       <c r="C34" s="29"/>
       <c r="D34" s="9" t="s">
@@ -1750,7 +1750,7 @@
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="6"/>
       <c r="C35" s="29"/>
       <c r="D35" s="9" t="s">
@@ -1767,7 +1767,7 @@
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="44"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="10"/>
       <c r="C36" s="30"/>
       <c r="D36" s="33" t="s">
@@ -1784,7 +1784,7 @@
       <c r="K36" s="5"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D40" s="48">
+      <c r="D40" s="37">
         <v>3665</v>
       </c>
       <c r="E40">
@@ -1881,7 +1881,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B7" s="48">
+      <c r="B7" s="37">
         <v>241</v>
       </c>
       <c r="C7">
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="AA9" s="48">
+      <c r="AA9" s="37">
         <v>241</v>
       </c>
     </row>

</xml_diff>